<commit_message>
Update Direcciones de memoria - PB.xlsx
</commit_message>
<xml_diff>
--- a/Documentación/Direcciones de memoria - PB.xlsx
+++ b/Documentación/Direcciones de memoria - PB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Macro Intell\sketchbook\Panic-Button\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0710FE41-F162-49F2-81F2-BB83D2923DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C050FF5E-2B1F-42F7-A271-E7FB3F93FD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Dirección</t>
   </si>
@@ -43,6 +43,42 @@
   </si>
   <si>
     <t>devID</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Destinatario 1</t>
+  </si>
+  <si>
+    <t>Destinatario 2</t>
+  </si>
+  <si>
+    <t>Destinatario 3</t>
+  </si>
+  <si>
+    <t>Firmware Versión</t>
+  </si>
+  <si>
+    <t>Hardware Versión</t>
+  </si>
+  <si>
+    <t>Si esta activado o no</t>
+  </si>
+  <si>
+    <t>devID del dispositivo</t>
   </si>
 </sst>
 </file>
@@ -382,18 +418,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -420,6 +456,9 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -431,40 +470,83 @@
       <c r="C3">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>